<commit_message>
commit 02 : update api export Information User
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/information_user.xlsx
+++ b/src/main/resources/excel/information_user.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Người xuất</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>{list.hoVaTen}</t>
+  </si>
+  <si>
+    <t>{list.username}</t>
   </si>
   <si>
     <t>{list.phoneNumber}</t>
@@ -120,11 +123,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy\ hh:mm"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -155,8 +158,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -164,60 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,53 +271,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -292,7 +295,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,19 +330,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,163 +414,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,35 +572,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -609,21 +583,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,156 +605,200 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1101,7 +1104,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1264,40 +1267,40 @@
         <v>21</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:14">

</xml_diff>

<commit_message>
Commit 04: update template excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/information_user.xlsx
+++ b/src/main/resources/excel/information_user.xlsx
@@ -123,13 +123,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy\ hh:mm"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -138,28 +138,153 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -167,99 +292,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,41 +307,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -330,19 +335,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,163 +515,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,21 +562,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -583,21 +573,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,9 +603,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,201 +659,190 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1104,7 +1109,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>